<commit_message>
use number rather than name
</commit_message>
<xml_diff>
--- a/mass_producer/生物.xlsx
+++ b/mass_producer/生物.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifeichen/WorkSpace/GithubRepos/Wizard-s-Deck/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifeichen/WorkSpace/GithubRepos/Wizard-s-Deck/mass_producer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65787EDF-D4BB-8A40-BEA3-3F69ABF8570D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7578E600-F9B0-A343-931F-325BCB7286AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="3000" windowWidth="28040" windowHeight="17260" xr2:uid="{58AF0140-36BA-C749-B66E-B595205C3BA3}"/>
+    <workbookView xWindow="680" yWindow="1860" windowWidth="28040" windowHeight="17260" xr2:uid="{58AF0140-36BA-C749-B66E-B595205C3BA3}"/>
   </bookViews>
   <sheets>
     <sheet name="火" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,6 +487,9 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>114514</v>
+      </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>

</xml_diff>